<commit_message>
Added new tab "minor correction"
</commit_message>
<xml_diff>
--- a/DataRe-Analysis/SummaryAnalysis_Dataset_v8.xlsx
+++ b/DataRe-Analysis/SummaryAnalysis_Dataset_v8.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13240" yWindow="0" windowWidth="17460" windowHeight="16040" tabRatio="954" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="0" windowWidth="26160" windowHeight="16160" tabRatio="954" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Antibodies-PRE" sheetId="15" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Figure 4" sheetId="16" r:id="rId8"/>
     <sheet name="binary significance test" sheetId="17" r:id="rId9"/>
     <sheet name="Correct usage" sheetId="20" r:id="rId10"/>
+    <sheet name="Minor Correction" sheetId="21" r:id="rId11"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8467" uniqueCount="1538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8476" uniqueCount="1540">
   <si>
     <t>Organisms</t>
   </si>
@@ -4946,6 +4947,12 @@
   </si>
   <si>
     <t>anti-bPIX (SH3 domain) from Millipore; anti-Î²-actin (catalog #ab66338 RRID:AB_2289239)</t>
+  </si>
+  <si>
+    <t>Minor correction (y)</t>
+  </si>
+  <si>
+    <t>Percent with minor correction</t>
   </si>
 </sst>
 </file>
@@ -5545,7 +5552,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1080">
+  <cellStyleXfs count="1100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="2" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -6277,6 +6284,26 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -7327,7 +7354,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1080">
+  <cellStyles count="1100">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -8229,6 +8256,16 @@
     <cellStyle name="Followed Hyperlink" xfId="1075" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1077" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1079" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1081" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1083" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1085" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1087" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1089" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1091" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1093" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1095" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1097" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1099" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="732" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="734" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="736" builtinId="8" hidden="1"/>
@@ -8403,6 +8440,16 @@
     <cellStyle name="Hyperlink" xfId="1074" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1076" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1078" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1080" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1082" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1084" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1086" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1088" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1090" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1092" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1094" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1096" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1098" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3"/>
     <cellStyle name="Normal 3" xfId="150"/>
@@ -15066,13 +15113,125 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="60"/>
+    <col min="2" max="3" width="10.83203125" style="90"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="60" t="s">
+        <v>1492</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="36">
+      <c r="A2" s="60" t="s">
+        <v>1419</v>
+      </c>
+      <c r="B2" s="90" t="s">
+        <v>1538</v>
+      </c>
+      <c r="C2" s="90" t="s">
+        <v>964</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="60" t="s">
+        <v>1483</v>
+      </c>
+      <c r="B3" s="90">
+        <f>'Antibody-POST 1st vs 2nd Abs'!G475</f>
+        <v>152</v>
+      </c>
+      <c r="C3" s="90">
+        <f>'Antibody-POST 1st vs 2nd Abs'!G476</f>
+        <v>429</v>
+      </c>
+      <c r="D3" s="154">
+        <f>B3/C3</f>
+        <v>0.35431235431235431</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="60" t="s">
+        <v>1359</v>
+      </c>
+      <c r="B4" s="90">
+        <f>'Organisms- POST'!G149</f>
+        <v>8</v>
+      </c>
+      <c r="C4" s="90">
+        <f>'Organisms- POST'!G150</f>
+        <v>54</v>
+      </c>
+      <c r="D4" s="154">
+        <f>B4/C4</f>
+        <v>0.14814814814814814</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="90">
+        <f>'Software- POST C v NC'!G111</f>
+        <v>26</v>
+      </c>
+      <c r="C5" s="90">
+        <f>'Software- POST C v NC'!G112</f>
+        <v>78</v>
+      </c>
+      <c r="D5" s="154">
+        <f>B5/C5</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="60" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B7" s="90">
+        <f>SUM(B3:B5)</f>
+        <v>186</v>
+      </c>
+      <c r="C7" s="90">
+        <f>SUM(C3:C5)</f>
+        <v>561</v>
+      </c>
+      <c r="D7" s="154">
+        <f>B7/C7</f>
+        <v>0.33155080213903743</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X485"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B59" sqref="B59:B70"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A469" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -29503,7 +29662,7 @@
       <c r="C453" s="165" t="s">
         <v>74</v>
       </c>
-      <c r="D453" s="62" t="s">
+      <c r="D453" s="172" t="s">
         <v>810</v>
       </c>
       <c r="E453" s="157" t="s">
@@ -32215,10 +32374,10 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K1014"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A148" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F148" sqref="F148:G151"/>
+      <selection pane="bottomLeft" activeCell="D143" sqref="B5:D143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
updated file based on conversation with MH and MB.
</commit_message>
<xml_diff>
--- a/DataRe-Analysis/SummaryAnalysis_Dataset_v8.xlsx
+++ b/DataRe-Analysis/SummaryAnalysis_Dataset_v8.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="0" windowWidth="26160" windowHeight="16160" tabRatio="954" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="3200" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="954" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Antibodies-PRE" sheetId="15" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8478" uniqueCount="1542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8479" uniqueCount="1543">
   <si>
     <t>Organisms</t>
   </si>
@@ -4960,6 +4960,9 @@
   </si>
   <si>
     <t>missing RRID prefix, should this be considered incorrect usage? Changed it to correct</t>
+  </si>
+  <si>
+    <t>(Syntactic Accuracy)</t>
   </si>
 </sst>
 </file>
@@ -5559,7 +5562,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1110">
+  <cellStyleXfs count="1124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="2" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -6291,6 +6294,20 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -7342,6 +7359,33 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="159" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="159" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="159" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="159" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="159" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="159" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="59" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="159" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7357,39 +7401,20 @@
     <xf numFmtId="0" fontId="46" fillId="9" borderId="1" xfId="150" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="159" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="72" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="159" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="159" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="159" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="159" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="59" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="159" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="16" borderId="1" xfId="159" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1110">
+  <cellStyles count="1124">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -8306,6 +8331,13 @@
     <cellStyle name="Followed Hyperlink" xfId="1105" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1107" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1123" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="732" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="734" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="736" builtinId="8" hidden="1"/>
@@ -8495,6 +8527,13 @@
     <cellStyle name="Hyperlink" xfId="1104" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1106" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1122" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3"/>
     <cellStyle name="Normal 3" xfId="150"/>
@@ -8657,11 +8696,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2145986936"/>
-        <c:axId val="2145990024"/>
+        <c:axId val="-2128803784"/>
+        <c:axId val="-2130583400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2145986936"/>
+        <c:axId val="-2128803784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8684,7 +8723,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2145990024"/>
+        <c:crossAx val="-2130583400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8692,7 +8731,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2145990024"/>
+        <c:axId val="-2130583400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -8716,7 +8755,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2145986936"/>
+        <c:crossAx val="-2128803784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -8965,11 +9004,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2142605688"/>
-        <c:axId val="2142602584"/>
+        <c:axId val="-2130637784"/>
+        <c:axId val="-2130640888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2142605688"/>
+        <c:axId val="-2130637784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8992,7 +9031,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142602584"/>
+        <c:crossAx val="-2130640888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9000,7 +9039,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2142602584"/>
+        <c:axId val="-2130640888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -9024,7 +9063,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142605688"/>
+        <c:crossAx val="-2130637784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -15273,9 +15312,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X486"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A468" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G473" sqref="G473"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -15361,7 +15400,9 @@
       <c r="G2" s="197" t="s">
         <v>1462</v>
       </c>
-      <c r="H2" s="197"/>
+      <c r="H2" s="197" t="s">
+        <v>1542</v>
+      </c>
       <c r="I2" s="179">
         <f>COUNTIF(I4:I475,"y")/COUNTA(I4:I475)</f>
         <v>0.96129032258064517</v>
@@ -16404,7 +16445,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="40" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B40" s="61">
         <v>24665018</v>
       </c>
@@ -16436,7 +16477,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="41" spans="2:11" s="144" customFormat="1" ht="33">
       <c r="B41" s="61">
         <v>24671998</v>
       </c>
@@ -16468,7 +16509,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="42" spans="2:11" s="144" customFormat="1" ht="33">
       <c r="B42" s="61">
         <v>24671998</v>
       </c>
@@ -16564,7 +16605,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="45" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B45" s="61">
         <v>24687876</v>
       </c>
@@ -16596,7 +16637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="46" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B46" s="61">
         <v>24687876</v>
       </c>
@@ -16658,7 +16699,7 @@
       </c>
       <c r="K47" s="157"/>
     </row>
-    <row r="48" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="48" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B48" s="61">
         <v>24715479</v>
       </c>
@@ -16690,7 +16731,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="49" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B49" s="61">
         <v>24715479</v>
       </c>
@@ -16914,7 +16955,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="2:11" s="144" customFormat="1" ht="13">
+    <row r="56" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B56" s="61">
         <v>24715505</v>
       </c>
@@ -16978,7 +17019,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="58" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B58" s="61">
         <v>24715505</v>
       </c>
@@ -17010,7 +17051,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="2:11" s="144" customFormat="1">
+    <row r="59" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B59" s="61">
         <v>24715505</v>
       </c>
@@ -17042,7 +17083,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="2:11" s="144" customFormat="1">
+    <row r="60" spans="2:11" s="144" customFormat="1" ht="22">
       <c r="B60" s="61">
         <v>24715528</v>
       </c>
@@ -17074,7 +17115,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="2:11" s="144" customFormat="1">
+    <row r="61" spans="2:11" s="144" customFormat="1" ht="22">
       <c r="B61" s="61">
         <v>24715528</v>
       </c>
@@ -17106,7 +17147,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="2:11" s="144" customFormat="1">
+    <row r="62" spans="2:11" s="144" customFormat="1" ht="33">
       <c r="B62" s="61">
         <v>24715528</v>
       </c>
@@ -17138,7 +17179,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="2:11" s="144" customFormat="1">
+    <row r="63" spans="2:11" s="144" customFormat="1" ht="22">
       <c r="B63" s="61">
         <v>24715528</v>
       </c>
@@ -17170,7 +17211,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="2:11" s="144" customFormat="1">
+    <row r="64" spans="2:11" s="144" customFormat="1" ht="22">
       <c r="B64" s="61">
         <v>24715528</v>
       </c>
@@ -17202,7 +17243,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:24" s="144" customFormat="1">
+    <row r="65" spans="1:24" s="144" customFormat="1" ht="22">
       <c r="B65" s="61">
         <v>24715528</v>
       </c>
@@ -17234,7 +17275,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:24" s="144" customFormat="1">
+    <row r="66" spans="1:24" s="144" customFormat="1" ht="22">
       <c r="B66" s="61">
         <v>24715528</v>
       </c>
@@ -17266,7 +17307,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:24" s="144" customFormat="1">
+    <row r="67" spans="1:24" s="144" customFormat="1" ht="22">
       <c r="B67" s="61">
         <v>24715528</v>
       </c>
@@ -17298,7 +17339,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:24" s="144" customFormat="1">
+    <row r="68" spans="1:24" s="144" customFormat="1" ht="22">
       <c r="B68" s="61">
         <v>24715528</v>
       </c>
@@ -17394,7 +17435,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:24" s="144" customFormat="1" ht="33">
+    <row r="71" spans="1:24" s="144" customFormat="1">
       <c r="B71" s="61">
         <v>24715575</v>
       </c>
@@ -17426,7 +17467,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:24" s="144" customFormat="1" ht="33">
+    <row r="72" spans="1:24" s="144" customFormat="1">
       <c r="B72" s="61">
         <v>24715575</v>
       </c>
@@ -17458,7 +17499,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="73" spans="1:24" s="144" customFormat="1">
       <c r="B73" s="61">
         <v>24715575</v>
       </c>
@@ -17554,7 +17595,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:24" s="144" customFormat="1" ht="48">
+    <row r="76" spans="1:24" s="144" customFormat="1">
       <c r="B76" s="61">
         <v>24737644</v>
       </c>
@@ -17586,7 +17627,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="77" spans="1:24" s="144" customFormat="1">
       <c r="B77" s="61">
         <v>24737644</v>
       </c>
@@ -17616,7 +17657,7 @@
       </c>
       <c r="K77" s="157"/>
     </row>
-    <row r="78" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="78" spans="1:24" s="144" customFormat="1">
       <c r="B78" s="61">
         <v>24737644</v>
       </c>
@@ -17648,7 +17689,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="79" spans="1:24" s="144" customFormat="1">
       <c r="B79" s="61">
         <v>24737644</v>
       </c>
@@ -17680,8 +17721,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:24" s="144" customFormat="1" ht="36">
-      <c r="A80" s="292" t="s">
+    <row r="80" spans="1:24" s="144" customFormat="1" ht="39">
+      <c r="A80" s="327" t="s">
         <v>1503</v>
       </c>
       <c r="B80" s="293">
@@ -17728,7 +17769,7 @@
       <c r="W80" s="292"/>
       <c r="X80" s="292"/>
     </row>
-    <row r="81" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="81" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B81" s="61">
         <v>24740429</v>
       </c>
@@ -17760,7 +17801,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="82" spans="2:11" s="144" customFormat="1">
       <c r="B82" s="61">
         <v>24752570</v>
       </c>
@@ -17792,7 +17833,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="83" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B83" s="61">
         <v>24752570</v>
       </c>
@@ -17856,7 +17897,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="85" spans="2:11" s="144" customFormat="1">
       <c r="B85" s="61">
         <v>24752570</v>
       </c>
@@ -17888,7 +17929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="86" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B86" s="61">
         <v>24752570</v>
       </c>
@@ -17920,7 +17961,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="87" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B87" s="61">
         <v>24752666</v>
       </c>
@@ -17952,7 +17993,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="88" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B88" s="61">
         <v>24752666</v>
       </c>
@@ -17984,7 +18025,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="89" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B89" s="61">
         <v>24752666</v>
       </c>
@@ -18016,7 +18057,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="90" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B90" s="61">
         <v>24752666</v>
       </c>
@@ -18048,7 +18089,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="91" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B91" s="61">
         <v>24752666</v>
       </c>
@@ -18080,7 +18121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="92" spans="2:11" s="144" customFormat="1">
       <c r="B92" s="61">
         <v>24752702</v>
       </c>
@@ -18112,7 +18153,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="93" spans="2:11" s="144" customFormat="1">
       <c r="B93" s="61">
         <v>24752702</v>
       </c>
@@ -18144,7 +18185,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="2:11" s="144" customFormat="1" ht="22">
+    <row r="94" spans="2:11" s="144" customFormat="1">
       <c r="B94" s="61">
         <v>24752702</v>
       </c>
@@ -18176,7 +18217,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="2:11" s="144" customFormat="1" ht="22">
+    <row r="95" spans="2:11" s="144" customFormat="1">
       <c r="B95" s="61">
         <v>24752702</v>
       </c>
@@ -18208,7 +18249,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="2:11" s="144" customFormat="1" ht="33">
+    <row r="96" spans="2:11" s="144" customFormat="1">
       <c r="B96" s="190">
         <v>24752702</v>
       </c>
@@ -18240,7 +18281,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="2:11" s="144" customFormat="1" ht="22">
+    <row r="97" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B97" s="61">
         <v>24760871</v>
       </c>
@@ -18272,7 +18313,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="2:11" s="144" customFormat="1" ht="22">
+    <row r="98" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B98" s="61">
         <v>24760871</v>
       </c>
@@ -18304,7 +18345,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="2:11" s="144" customFormat="1" ht="22">
+    <row r="99" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B99" s="61">
         <v>24760871</v>
       </c>
@@ -18336,7 +18377,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="2:11" s="144" customFormat="1" ht="22">
+    <row r="100" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B100" s="61">
         <v>24760871</v>
       </c>
@@ -18368,7 +18409,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="2:11" s="144" customFormat="1" ht="22">
+    <row r="101" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B101" s="61">
         <v>24760871</v>
       </c>
@@ -18400,7 +18441,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="2:11" s="144" customFormat="1" ht="22">
+    <row r="102" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B102" s="61">
         <v>24760871</v>
       </c>
@@ -18432,7 +18473,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="2:11" s="144" customFormat="1" ht="13">
+    <row r="103" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B103" s="61">
         <v>24760871</v>
       </c>
@@ -18464,7 +18505,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="2:11" s="144" customFormat="1">
+    <row r="104" spans="2:11" s="144" customFormat="1" ht="44">
       <c r="B104" s="61">
         <v>24760871</v>
       </c>
@@ -18496,7 +18537,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="2:11" s="144" customFormat="1">
+    <row r="105" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B105" s="61">
         <v>24760871</v>
       </c>
@@ -18528,7 +18569,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="106" spans="2:11" s="144" customFormat="1">
+    <row r="106" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B106" s="61">
         <v>24760871</v>
       </c>
@@ -18560,7 +18601,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="2:11" s="144" customFormat="1">
+    <row r="107" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B107" s="61">
         <v>24771457</v>
       </c>
@@ -18592,7 +18633,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="2:11" s="144" customFormat="1">
+    <row r="108" spans="2:11" s="144" customFormat="1" ht="48">
       <c r="B108" s="61">
         <v>24771457</v>
       </c>
@@ -18624,7 +18665,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="109" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B109" s="61">
         <v>24771457</v>
       </c>
@@ -18656,7 +18697,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="110" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B110" s="61">
         <v>24771457</v>
       </c>
@@ -18688,7 +18729,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="2:11" s="144" customFormat="1">
+    <row r="111" spans="2:11" s="144" customFormat="1" ht="60">
       <c r="B111" s="61">
         <v>24782245</v>
       </c>
@@ -18718,7 +18759,7 @@
       </c>
       <c r="K111" s="157"/>
     </row>
-    <row r="112" spans="2:11" s="144" customFormat="1">
+    <row r="112" spans="2:11" s="144" customFormat="1" ht="60">
       <c r="B112" s="61">
         <v>24782245</v>
       </c>
@@ -18750,7 +18791,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="1:24" s="144" customFormat="1">
+    <row r="113" spans="1:24" s="144" customFormat="1" ht="36">
       <c r="B113" s="61">
         <v>24782245</v>
       </c>
@@ -18782,7 +18823,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:24" s="144" customFormat="1">
+    <row r="114" spans="1:24" s="144" customFormat="1" ht="72">
       <c r="B114" s="61">
         <v>24782245</v>
       </c>
@@ -18814,7 +18855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:24" s="292" customFormat="1" ht="13">
+    <row r="115" spans="1:24" s="292" customFormat="1" ht="36">
       <c r="A115" s="144"/>
       <c r="B115" s="61">
         <v>24782245</v>
@@ -18860,7 +18901,7 @@
       <c r="W115" s="144"/>
       <c r="X115" s="144"/>
     </row>
-    <row r="116" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="116" spans="1:24" s="144" customFormat="1" ht="65">
       <c r="A116" s="292" t="s">
         <v>1505</v>
       </c>
@@ -18870,7 +18911,7 @@
       <c r="C116" s="297" t="s">
         <v>25</v>
       </c>
-      <c r="D116" s="325" t="s">
+      <c r="D116" s="317" t="s">
         <v>1504</v>
       </c>
       <c r="E116" s="295" t="s">
@@ -18908,7 +18949,7 @@
       <c r="W116" s="292"/>
       <c r="X116" s="292"/>
     </row>
-    <row r="117" spans="1:24" s="144" customFormat="1">
+    <row r="117" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B117" s="61">
         <v>24790185</v>
       </c>
@@ -19004,7 +19045,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:24" s="144" customFormat="1">
+    <row r="120" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B120" s="61">
         <v>24790185</v>
       </c>
@@ -19036,7 +19077,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="121" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B121" s="61">
         <v>24790185</v>
       </c>
@@ -19068,7 +19109,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="122" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="122" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B122" s="61">
         <v>24790185</v>
       </c>
@@ -19100,7 +19141,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="123" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B123" s="61">
         <v>24790185</v>
       </c>
@@ -19132,7 +19173,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="124" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B124" s="61">
         <v>24790185</v>
       </c>
@@ -19164,7 +19205,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="125" spans="1:24" s="144" customFormat="1">
       <c r="B125" s="61">
         <v>24825750</v>
       </c>
@@ -19196,7 +19237,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="126" spans="1:24" s="144" customFormat="1">
       <c r="B126" s="61">
         <v>24825750</v>
       </c>
@@ -19228,7 +19269,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="127" spans="1:24" s="144" customFormat="1">
       <c r="B127" s="61">
         <v>24825750</v>
       </c>
@@ -19420,7 +19461,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="133" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="133" spans="2:11" s="144" customFormat="1">
       <c r="B133" s="190">
         <v>24825750</v>
       </c>
@@ -19452,7 +19493,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="134" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="134" spans="2:11" s="144" customFormat="1">
       <c r="B134" s="190">
         <v>24825750</v>
       </c>
@@ -19484,7 +19525,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="135" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="135" spans="2:11" s="144" customFormat="1">
       <c r="B135" s="190">
         <v>24825750</v>
       </c>
@@ -19516,7 +19557,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="136" spans="2:11" s="144" customFormat="1">
       <c r="B136" s="190">
         <v>24825750</v>
       </c>
@@ -19548,7 +19589,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="137" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="137" spans="2:11" s="144" customFormat="1" ht="48">
       <c r="B137" s="190">
         <v>24825798</v>
       </c>
@@ -19610,7 +19651,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="139" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="139" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B139" s="190">
         <v>24849359</v>
       </c>
@@ -19642,7 +19683,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="140" spans="2:11" s="144" customFormat="1" ht="44">
+    <row r="140" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B140" s="190">
         <v>24849359</v>
       </c>
@@ -19674,7 +19715,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="141" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="141" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B141" s="190">
         <v>24849359</v>
       </c>
@@ -19770,7 +19811,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="2:11" s="144" customFormat="1" ht="48">
+    <row r="144" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B144" s="190">
         <v>24899700</v>
       </c>
@@ -19866,7 +19907,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="147" spans="1:24" s="144" customFormat="1" ht="60">
+    <row r="147" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B147" s="61">
         <v>24899700</v>
       </c>
@@ -19898,7 +19939,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="148" spans="1:24" s="144" customFormat="1" ht="60">
+    <row r="148" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B148" s="61">
         <v>24899700</v>
       </c>
@@ -19930,7 +19971,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="149" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="149" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B149" s="190">
         <v>24899700</v>
       </c>
@@ -19962,7 +20003,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="150" spans="1:24" s="144" customFormat="1" ht="72">
+    <row r="150" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B150" s="190">
         <v>24899700</v>
       </c>
@@ -19994,7 +20035,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="151" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="151" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B151" s="190">
         <v>24899700</v>
       </c>
@@ -20026,7 +20067,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="152" spans="1:24" s="292" customFormat="1" ht="65">
+    <row r="152" spans="1:24" s="292" customFormat="1" ht="24">
       <c r="A152" s="144"/>
       <c r="B152" s="183">
         <v>24920616</v>
@@ -20072,7 +20113,7 @@
       <c r="W152" s="144"/>
       <c r="X152" s="144"/>
     </row>
-    <row r="153" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="153" spans="1:24" s="144" customFormat="1" ht="48">
       <c r="B153" s="61">
         <v>24920620</v>
       </c>
@@ -20168,7 +20209,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="156" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="156" spans="1:24" s="144" customFormat="1" ht="36">
       <c r="B156" s="61">
         <v>24920620</v>
       </c>
@@ -20264,7 +20305,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="159" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="159" spans="1:24" s="144" customFormat="1" ht="36">
       <c r="B159" s="61">
         <v>24920620</v>
       </c>
@@ -20360,7 +20401,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="162" spans="2:11" s="144" customFormat="1">
+    <row r="162" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B162" s="61">
         <v>24920620</v>
       </c>
@@ -20392,7 +20433,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="163" spans="2:11" s="144" customFormat="1">
+    <row r="163" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B163" s="61">
         <v>24920620</v>
       </c>
@@ -20424,7 +20465,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="164" spans="2:11" s="144" customFormat="1">
+    <row r="164" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B164" s="61">
         <v>24920620</v>
       </c>
@@ -20456,7 +20497,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="165" spans="2:11" s="144" customFormat="1">
+    <row r="165" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B165" s="61">
         <v>24920620</v>
       </c>
@@ -20488,7 +20529,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="166" spans="2:11" s="144" customFormat="1">
+    <row r="166" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B166" s="61">
         <v>24920620</v>
       </c>
@@ -20520,7 +20561,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="167" spans="2:11" s="144" customFormat="1">
+    <row r="167" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B167" s="61">
         <v>24920620</v>
       </c>
@@ -20552,7 +20593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="168" spans="2:11" s="144" customFormat="1">
+    <row r="168" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B168" s="183">
         <v>24920622</v>
       </c>
@@ -20584,7 +20625,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="169" spans="2:11" s="144" customFormat="1">
+    <row r="169" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B169" s="183">
         <v>24920622</v>
       </c>
@@ -20616,7 +20657,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="170" spans="2:11" s="144" customFormat="1">
+    <row r="170" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B170" s="183">
         <v>24920622</v>
       </c>
@@ -20648,7 +20689,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="171" spans="2:11" s="144" customFormat="1">
+    <row r="171" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B171" s="183">
         <v>24920622</v>
       </c>
@@ -20680,7 +20721,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="172" spans="2:11" s="144" customFormat="1">
+    <row r="172" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B172" s="183">
         <v>24920622</v>
       </c>
@@ -20712,7 +20753,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="173" spans="2:11" s="144" customFormat="1">
+    <row r="173" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B173" s="183">
         <v>24920622</v>
       </c>
@@ -20776,14 +20817,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="175" spans="2:11" s="144" customFormat="1">
+    <row r="175" spans="2:11" s="144" customFormat="1" ht="33">
       <c r="B175" s="183">
         <v>24920622</v>
       </c>
       <c r="C175" s="165" t="s">
         <v>2</v>
       </c>
-      <c r="D175" s="327" t="s">
+      <c r="D175" s="318" t="s">
         <v>736</v>
       </c>
       <c r="E175" s="61" t="s">
@@ -20806,7 +20847,7 @@
       </c>
       <c r="K175" s="157"/>
     </row>
-    <row r="176" spans="2:11" s="144" customFormat="1">
+    <row r="176" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B176" s="183">
         <v>24920622</v>
       </c>
@@ -20838,7 +20879,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="177" spans="1:24" s="144" customFormat="1">
+    <row r="177" spans="1:24" s="144" customFormat="1" ht="36">
       <c r="B177" s="183">
         <v>24920622</v>
       </c>
@@ -20870,7 +20911,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="178" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="178" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B178" s="183">
         <v>24920622</v>
       </c>
@@ -20934,7 +20975,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="180" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="180" spans="1:24" s="144" customFormat="1" ht="36">
       <c r="B180" s="183">
         <v>24920622</v>
       </c>
@@ -21030,7 +21071,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="183" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="183" spans="1:24" s="144" customFormat="1" ht="36">
       <c r="B183" s="61">
         <v>24920622</v>
       </c>
@@ -21062,7 +21103,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="184" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="184" spans="1:24" s="144" customFormat="1" ht="33">
       <c r="B184" s="61">
         <v>24920622</v>
       </c>
@@ -21094,7 +21135,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="185" spans="1:24" s="144" customFormat="1" ht="60">
+    <row r="185" spans="1:24" s="144" customFormat="1" ht="33">
       <c r="B185" s="61">
         <v>24920622</v>
       </c>
@@ -21126,7 +21167,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="186" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="186" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B186" s="61">
         <v>24920622</v>
       </c>
@@ -21190,7 +21231,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="188" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="188" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="A188" s="292" t="s">
         <v>1505</v>
       </c>
@@ -21245,7 +21286,7 @@
       <c r="C189" s="165" t="s">
         <v>25</v>
       </c>
-      <c r="D189" s="319" t="s">
+      <c r="D189" s="312" t="s">
         <v>720</v>
       </c>
       <c r="E189" s="61" t="s">
@@ -21270,14 +21311,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="190" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="190" spans="1:24" s="144" customFormat="1" ht="36">
       <c r="B190" s="61">
         <v>24942187</v>
       </c>
       <c r="C190" s="165" t="s">
         <v>25</v>
       </c>
-      <c r="D190" s="319" t="s">
+      <c r="D190" s="312" t="s">
         <v>721</v>
       </c>
       <c r="E190" s="61" t="s">
@@ -21430,7 +21471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="195" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="195" spans="1:24" s="144" customFormat="1" ht="33">
       <c r="B195" s="61">
         <v>24966380</v>
       </c>
@@ -21494,7 +21535,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="197" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="197" spans="1:24" s="144" customFormat="1" ht="36">
       <c r="B197" s="61">
         <v>24966384</v>
       </c>
@@ -21526,7 +21567,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="198" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="198" spans="1:24" s="144" customFormat="1" ht="36">
       <c r="B198" s="61">
         <v>24966384</v>
       </c>
@@ -21558,7 +21599,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="199" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="199" spans="1:24" s="144" customFormat="1" ht="36">
       <c r="B199" s="61">
         <v>24966384</v>
       </c>
@@ -21622,7 +21663,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="201" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="201" spans="1:24" s="144" customFormat="1" ht="36">
       <c r="B201" s="61">
         <v>24966384</v>
       </c>
@@ -21750,7 +21791,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="205" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="205" spans="1:24" s="144" customFormat="1" ht="39">
       <c r="B205" s="61">
         <v>24966384</v>
       </c>
@@ -21780,7 +21821,7 @@
       </c>
       <c r="K205" s="157"/>
     </row>
-    <row r="206" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="206" spans="1:24" s="144" customFormat="1" ht="48">
       <c r="A206" s="292" t="s">
         <v>1510</v>
       </c>
@@ -21828,7 +21869,7 @@
       <c r="W206" s="292"/>
       <c r="X206" s="292"/>
     </row>
-    <row r="207" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="207" spans="1:24" s="144" customFormat="1" ht="48">
       <c r="B207" s="61">
         <v>24984694</v>
       </c>
@@ -21892,7 +21933,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="209" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="209" spans="1:24" s="144" customFormat="1" ht="60">
       <c r="B209" s="61">
         <v>24984694</v>
       </c>
@@ -21922,7 +21963,7 @@
       </c>
       <c r="K209" s="163"/>
     </row>
-    <row r="210" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="210" spans="1:24" s="144" customFormat="1" ht="48">
       <c r="B210" s="61">
         <v>24984694</v>
       </c>
@@ -21954,7 +21995,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="211" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="211" spans="1:24" s="144" customFormat="1">
       <c r="A211" s="292" t="s">
         <v>1505</v>
       </c>
@@ -21964,7 +22005,7 @@
       <c r="C211" s="269" t="s">
         <v>2</v>
       </c>
-      <c r="D211" s="313" t="s">
+      <c r="D211" s="308" t="s">
         <v>1522</v>
       </c>
       <c r="E211" s="269" t="s">
@@ -22002,7 +22043,7 @@
       <c r="W211" s="292"/>
       <c r="X211" s="292"/>
     </row>
-    <row r="212" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="212" spans="1:24" s="144" customFormat="1">
       <c r="A212" s="292" t="s">
         <v>1505</v>
       </c>
@@ -22012,7 +22053,7 @@
       <c r="C212" s="269" t="s">
         <v>2</v>
       </c>
-      <c r="D212" s="313" t="s">
+      <c r="D212" s="308" t="s">
         <v>1523</v>
       </c>
       <c r="E212" s="269" t="s">
@@ -22050,7 +22091,7 @@
       <c r="W212" s="292"/>
       <c r="X212" s="292"/>
     </row>
-    <row r="213" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="213" spans="1:24" s="144" customFormat="1">
       <c r="A213" s="292" t="s">
         <v>1505</v>
       </c>
@@ -22060,7 +22101,7 @@
       <c r="C213" s="269" t="s">
         <v>2</v>
       </c>
-      <c r="D213" s="313" t="s">
+      <c r="D213" s="308" t="s">
         <v>1524</v>
       </c>
       <c r="E213" s="269" t="s">
@@ -22098,7 +22139,7 @@
       <c r="W213" s="292"/>
       <c r="X213" s="292"/>
     </row>
-    <row r="214" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="214" spans="1:24" s="144" customFormat="1">
       <c r="A214" s="292" t="s">
         <v>1505</v>
       </c>
@@ -22108,7 +22149,7 @@
       <c r="C214" s="269" t="s">
         <v>2</v>
       </c>
-      <c r="D214" s="313" t="s">
+      <c r="D214" s="308" t="s">
         <v>1525</v>
       </c>
       <c r="E214" s="269" t="s">
@@ -22146,7 +22187,7 @@
       <c r="W214" s="292"/>
       <c r="X214" s="292"/>
     </row>
-    <row r="215" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="215" spans="1:24" s="144" customFormat="1">
       <c r="A215" s="292" t="s">
         <v>1505</v>
       </c>
@@ -22156,7 +22197,7 @@
       <c r="C215" s="269" t="s">
         <v>2</v>
       </c>
-      <c r="D215" s="313" t="s">
+      <c r="D215" s="308" t="s">
         <v>1526</v>
       </c>
       <c r="E215" s="269" t="s">
@@ -22194,17 +22235,17 @@
       <c r="W215" s="292"/>
       <c r="X215" s="292"/>
     </row>
-    <row r="216" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="216" spans="1:24" s="144" customFormat="1">
       <c r="A216" s="292" t="s">
         <v>1505</v>
       </c>
-      <c r="B216" s="313">
+      <c r="B216" s="308">
         <v>24990930</v>
       </c>
-      <c r="C216" s="313" t="s">
+      <c r="C216" s="308" t="s">
         <v>2</v>
       </c>
-      <c r="D216" s="313" t="s">
+      <c r="D216" s="308" t="s">
         <v>1527</v>
       </c>
       <c r="E216" s="269" t="s">
@@ -22281,7 +22322,7 @@
       <c r="C218" s="178" t="s">
         <v>2</v>
       </c>
-      <c r="D218" s="313" t="s">
+      <c r="D218" s="308" t="s">
         <v>1528</v>
       </c>
       <c r="E218" s="178" t="s">
@@ -22338,7 +22379,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="220" spans="1:24" s="144" customFormat="1" ht="60">
+    <row r="220" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B220" s="62">
         <v>25009260</v>
       </c>
@@ -22370,7 +22411,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="221" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="221" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B221" s="62">
         <v>25009260</v>
       </c>
@@ -22466,7 +22507,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="224" spans="1:24" s="292" customFormat="1" ht="36">
+    <row r="224" spans="1:24" s="292" customFormat="1" ht="24">
       <c r="A224" s="144"/>
       <c r="B224" s="62">
         <v>25009260</v>
@@ -22512,14 +22553,14 @@
       <c r="W224" s="144"/>
       <c r="X224" s="144"/>
     </row>
-    <row r="225" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="225" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B225" s="62">
         <v>25009260</v>
       </c>
       <c r="C225" s="178" t="s">
         <v>2</v>
       </c>
-      <c r="D225" s="318" t="s">
+      <c r="D225" s="311" t="s">
         <v>671</v>
       </c>
       <c r="E225" s="178" t="s">
@@ -22608,7 +22649,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="228" spans="1:24" s="144" customFormat="1" ht="13">
+    <row r="228" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B228" s="62">
         <v>25009276</v>
       </c>
@@ -22640,7 +22681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="229" spans="1:24" s="292" customFormat="1" ht="13">
+    <row r="229" spans="1:24" s="292" customFormat="1" ht="24">
       <c r="A229" s="144"/>
       <c r="B229" s="62">
         <v>25009276</v>
@@ -22648,7 +22689,7 @@
       <c r="C229" s="178" t="s">
         <v>2</v>
       </c>
-      <c r="D229" s="316" t="s">
+      <c r="D229" s="310" t="s">
         <v>674</v>
       </c>
       <c r="E229" s="178" t="s">
@@ -22686,7 +22727,7 @@
       <c r="W229" s="144"/>
       <c r="X229" s="144"/>
     </row>
-    <row r="230" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="230" spans="1:24" s="144" customFormat="1" ht="36">
       <c r="B230" s="62">
         <v>25009276</v>
       </c>
@@ -22782,7 +22823,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="233" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="233" spans="1:24" s="144" customFormat="1" ht="36">
       <c r="B233" s="62">
         <v>25009276</v>
       </c>
@@ -22878,7 +22919,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="236" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="236" spans="1:24" s="144" customFormat="1" ht="36">
       <c r="B236" s="62">
         <v>25009276</v>
       </c>
@@ -22942,7 +22983,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="238" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="238" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B238" s="62">
         <v>25009276</v>
       </c>
@@ -22974,7 +23015,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="239" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="239" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B239" s="62">
         <v>25009276</v>
       </c>
@@ -23070,7 +23111,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="242" spans="2:11" s="144" customFormat="1" ht="48">
+    <row r="242" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B242" s="61">
         <v>25031405</v>
       </c>
@@ -23102,7 +23143,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="243" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="243" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B243" s="61">
         <v>25031414</v>
       </c>
@@ -23134,7 +23175,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="244" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="244" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B244" s="61">
         <v>25031414</v>
       </c>
@@ -23166,7 +23207,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="245" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="245" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B245" s="61">
         <v>25031414</v>
       </c>
@@ -23198,7 +23239,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="246" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="246" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B246" s="61">
         <v>25031414</v>
       </c>
@@ -23230,7 +23271,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="247" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="247" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B247" s="61">
         <v>25031414</v>
       </c>
@@ -23262,7 +23303,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="248" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="248" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B248" s="61">
         <v>25031414</v>
       </c>
@@ -23422,7 +23463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="253" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="253" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B253" s="61">
         <v>25031414</v>
       </c>
@@ -23486,7 +23527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="255" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="255" spans="2:11" s="144" customFormat="1" ht="26">
       <c r="B255" s="62">
         <v>25043933</v>
       </c>
@@ -23518,7 +23559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="256" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="256" spans="2:11" s="144" customFormat="1" ht="26">
       <c r="B256" s="62">
         <v>25043933</v>
       </c>
@@ -23550,7 +23591,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="257" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="257" spans="2:11" s="144" customFormat="1" ht="26">
       <c r="B257" s="62">
         <v>25043933</v>
       </c>
@@ -23582,7 +23623,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="258" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="258" spans="2:11" s="144" customFormat="1" ht="26">
       <c r="B258" s="62">
         <v>25043933</v>
       </c>
@@ -23614,7 +23655,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="259" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="259" spans="2:11" s="144" customFormat="1" ht="39">
       <c r="B259" s="62">
         <v>25043933</v>
       </c>
@@ -23646,7 +23687,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="260" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="260" spans="2:11" s="144" customFormat="1" ht="26">
       <c r="B260" s="62">
         <v>25043933</v>
       </c>
@@ -23678,7 +23719,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="261" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="261" spans="2:11" s="144" customFormat="1" ht="26">
       <c r="B261" s="62">
         <v>25043933</v>
       </c>
@@ -23710,7 +23751,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="262" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="262" spans="2:11" s="144" customFormat="1" ht="26">
       <c r="B262" s="62">
         <v>25043933</v>
       </c>
@@ -23742,7 +23783,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="263" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="263" spans="2:11" s="144" customFormat="1" ht="26">
       <c r="B263" s="62">
         <v>25043933</v>
       </c>
@@ -23774,7 +23815,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="264" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="264" spans="2:11" s="144" customFormat="1" ht="26">
       <c r="B264" s="62">
         <v>25043933</v>
       </c>
@@ -23806,7 +23847,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="265" spans="2:11" s="144" customFormat="1" ht="48">
+    <row r="265" spans="2:11" s="144" customFormat="1" ht="26">
       <c r="B265" s="62">
         <v>25043933</v>
       </c>
@@ -23838,7 +23879,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="266" spans="2:11" s="144" customFormat="1" ht="33">
+    <row r="266" spans="2:11" s="144" customFormat="1" ht="48">
       <c r="B266" s="61">
         <v>25044160</v>
       </c>
@@ -23934,7 +23975,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="269" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="269" spans="2:11" s="144" customFormat="1" ht="48">
       <c r="B269" s="61">
         <v>25044160</v>
       </c>
@@ -23966,7 +24007,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="270" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="270" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B270" s="61">
         <v>25080583</v>
       </c>
@@ -24126,7 +24167,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="275" spans="1:24" s="144" customFormat="1" ht="33">
+    <row r="275" spans="1:24" s="144" customFormat="1" ht="36">
       <c r="B275" s="61">
         <v>25100594</v>
       </c>
@@ -24158,7 +24199,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="276" spans="1:24" s="144" customFormat="1" ht="33">
+    <row r="276" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B276" s="61">
         <v>25100594</v>
       </c>
@@ -24222,7 +24263,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="278" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="278" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B278" s="61">
         <v>25100594</v>
       </c>
@@ -24300,7 +24341,7 @@
       <c r="W279" s="144"/>
       <c r="X279" s="144"/>
     </row>
-    <row r="280" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="280" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B280" s="61">
         <v>25100594</v>
       </c>
@@ -24332,7 +24373,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="281" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="281" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B281" s="61">
         <v>25100594</v>
       </c>
@@ -24364,7 +24405,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="282" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="282" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B282" s="61">
         <v>25100594</v>
       </c>
@@ -24396,7 +24437,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="283" spans="1:24" s="144" customFormat="1">
+    <row r="283" spans="1:24" s="144" customFormat="1" ht="36">
       <c r="B283" s="61">
         <v>25100594</v>
       </c>
@@ -24428,7 +24469,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="284" spans="1:24" s="144" customFormat="1" ht="26">
+    <row r="284" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B284" s="61">
         <v>25100594</v>
       </c>
@@ -24460,7 +24501,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="285" spans="1:24" s="144" customFormat="1" ht="26">
+    <row r="285" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B285" s="61">
         <v>25100604</v>
       </c>
@@ -24492,7 +24533,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="286" spans="1:24" s="144" customFormat="1" ht="26">
+    <row r="286" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B286" s="61">
         <v>25100604</v>
       </c>
@@ -24524,7 +24565,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="287" spans="1:24" s="144" customFormat="1" ht="39">
+    <row r="287" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B287" s="61">
         <v>25100604</v>
       </c>
@@ -24556,7 +24597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="288" spans="1:24" s="144" customFormat="1">
+    <row r="288" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B288" s="61">
         <v>25100604</v>
       </c>
@@ -24588,7 +24629,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="289" spans="2:11" s="144" customFormat="1" ht="48">
+    <row r="289" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B289" s="61">
         <v>25100604</v>
       </c>
@@ -24620,7 +24661,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="290" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="290" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B290" s="190">
         <v>25100604</v>
       </c>
@@ -24716,7 +24757,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="293" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="293" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B293" s="190">
         <v>25100604</v>
       </c>
@@ -24748,7 +24789,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="294" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="294" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B294" s="190">
         <v>25100604</v>
       </c>
@@ -24780,7 +24821,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="295" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="295" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B295" s="190">
         <v>25100604</v>
       </c>
@@ -24812,7 +24853,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="296" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="296" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B296" s="190">
         <v>25100604</v>
       </c>
@@ -24844,7 +24885,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="297" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="297" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B297" s="190">
         <v>25100604</v>
       </c>
@@ -24972,14 +25013,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="301" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="301" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B301" s="221">
         <v>25177484</v>
       </c>
       <c r="C301" s="165" t="s">
         <v>74</v>
       </c>
-      <c r="D301" s="321" t="s">
+      <c r="D301" s="314" t="s">
         <v>810</v>
       </c>
       <c r="E301" s="157" t="s">
@@ -25068,7 +25109,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="304" spans="2:11" s="144" customFormat="1" ht="48">
+    <row r="304" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B304" s="221">
         <v>25177484</v>
       </c>
@@ -25132,7 +25173,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="306" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="306" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B306" s="221">
         <v>25177484</v>
       </c>
@@ -25196,7 +25237,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="308" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="308" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B308" s="221">
         <v>25177484</v>
       </c>
@@ -25260,7 +25301,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="310" spans="2:11" s="144" customFormat="1" ht="33">
+    <row r="310" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B310" s="221">
         <v>25202271</v>
       </c>
@@ -25292,7 +25333,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="311" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="311" spans="2:11" s="144" customFormat="1" ht="48">
       <c r="B311" s="221">
         <v>25202271</v>
       </c>
@@ -25420,7 +25461,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="315" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="315" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B315" s="221">
         <v>25202271</v>
       </c>
@@ -25580,7 +25621,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="320" spans="2:11" s="144" customFormat="1" ht="39">
+    <row r="320" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B320" s="61">
         <v>24659141</v>
       </c>
@@ -25612,7 +25653,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="321" spans="1:24" s="292" customFormat="1" ht="48">
+    <row r="321" spans="1:24" s="292" customFormat="1" ht="24">
       <c r="A321" s="144"/>
       <c r="B321" s="61">
         <v>24659141</v>
@@ -25658,7 +25699,7 @@
       <c r="W321" s="144"/>
       <c r="X321" s="144"/>
     </row>
-    <row r="322" spans="1:24" s="144" customFormat="1" ht="48">
+    <row r="322" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B322" s="61">
         <v>24659141</v>
       </c>
@@ -25722,7 +25763,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="324" spans="1:24" s="144" customFormat="1" ht="60">
+    <row r="324" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B324" s="61">
         <v>24659141</v>
       </c>
@@ -25754,7 +25795,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="325" spans="1:24" s="144" customFormat="1" ht="48">
+    <row r="325" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B325" s="61">
         <v>24659141</v>
       </c>
@@ -25786,7 +25827,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="326" spans="1:24" s="144" customFormat="1" ht="13">
+    <row r="326" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B326" s="183">
         <v>24659141</v>
       </c>
@@ -25818,7 +25859,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="327" spans="1:24" s="144" customFormat="1" ht="13">
+    <row r="327" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B327" s="183">
         <v>24659141</v>
       </c>
@@ -25850,7 +25891,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="328" spans="1:24" s="144" customFormat="1" ht="13">
+    <row r="328" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B328" s="183">
         <v>24659141</v>
       </c>
@@ -25882,7 +25923,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="329" spans="1:24" s="144" customFormat="1" ht="52">
+    <row r="329" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B329" s="183">
         <v>24659141</v>
       </c>
@@ -25914,7 +25955,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="330" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="330" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B330" s="183">
         <v>24659141</v>
       </c>
@@ -25978,7 +26019,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="332" spans="1:24" s="292" customFormat="1">
+    <row r="332" spans="1:24" s="292" customFormat="1" ht="24">
       <c r="A332" s="144"/>
       <c r="B332" s="183">
         <v>24659141</v>
@@ -26024,7 +26065,7 @@
       <c r="W332" s="144"/>
       <c r="X332" s="144"/>
     </row>
-    <row r="333" spans="1:24" s="292" customFormat="1">
+    <row r="333" spans="1:24" s="292" customFormat="1" ht="13">
       <c r="A333" s="144"/>
       <c r="B333" s="183">
         <v>24659141</v>
@@ -26032,7 +26073,7 @@
       <c r="C333" s="290" t="s">
         <v>25</v>
       </c>
-      <c r="D333" s="323" t="s">
+      <c r="D333" s="316" t="s">
         <v>1407</v>
       </c>
       <c r="E333" s="159" t="s">
@@ -26070,7 +26111,7 @@
       <c r="W333" s="144"/>
       <c r="X333" s="144"/>
     </row>
-    <row r="334" spans="1:24" s="292" customFormat="1">
+    <row r="334" spans="1:24" s="292" customFormat="1" ht="24">
       <c r="A334" s="144"/>
       <c r="B334" s="183">
         <v>24659141</v>
@@ -26124,7 +26165,7 @@
       <c r="C335" s="290" t="s">
         <v>25</v>
       </c>
-      <c r="D335" s="314" t="s">
+      <c r="D335" s="309" t="s">
         <v>928</v>
       </c>
       <c r="E335" s="61" t="s">
@@ -26170,7 +26211,7 @@
       <c r="C336" s="290" t="s">
         <v>25</v>
       </c>
-      <c r="D336" s="314" t="s">
+      <c r="D336" s="309" t="s">
         <v>929</v>
       </c>
       <c r="E336" s="61" t="s">
@@ -26216,7 +26257,7 @@
       <c r="C337" s="290" t="s">
         <v>25</v>
       </c>
-      <c r="D337" s="314" t="s">
+      <c r="D337" s="309" t="s">
         <v>915</v>
       </c>
       <c r="E337" s="61" t="s">
@@ -26254,7 +26295,7 @@
       <c r="W337" s="144"/>
       <c r="X337" s="144"/>
     </row>
-    <row r="338" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="338" spans="1:24" s="144" customFormat="1">
       <c r="B338" s="61">
         <v>24668417</v>
       </c>
@@ -26286,14 +26327,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="339" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="339" spans="1:24" s="144" customFormat="1">
       <c r="B339" s="61">
         <v>24668417</v>
       </c>
       <c r="C339" s="165" t="s">
         <v>25</v>
       </c>
-      <c r="D339" s="314" t="s">
+      <c r="D339" s="309" t="s">
         <v>917</v>
       </c>
       <c r="E339" s="61" t="s">
@@ -26318,7 +26359,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="340" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="340" spans="1:24" s="144" customFormat="1">
       <c r="B340" s="61">
         <v>24668417</v>
       </c>
@@ -26350,7 +26391,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="341" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="341" spans="1:24" s="144" customFormat="1">
       <c r="B341" s="61">
         <v>24668417</v>
       </c>
@@ -26382,7 +26423,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="342" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="342" spans="1:24" s="144" customFormat="1">
       <c r="B342" s="61">
         <v>24668417</v>
       </c>
@@ -26414,7 +26455,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="343" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="343" spans="1:24" s="144" customFormat="1">
       <c r="B343" s="61">
         <v>24668417</v>
       </c>
@@ -26446,7 +26487,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="344" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="344" spans="1:24" s="144" customFormat="1">
       <c r="B344" s="61">
         <v>24668417</v>
       </c>
@@ -26478,7 +26519,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="345" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="345" spans="1:24" s="144" customFormat="1">
       <c r="B345" s="61">
         <v>24668417</v>
       </c>
@@ -26510,7 +26551,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="346" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="346" spans="1:24" s="144" customFormat="1">
       <c r="B346" s="61">
         <v>24668417</v>
       </c>
@@ -26542,7 +26583,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="347" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="347" spans="1:24" s="144" customFormat="1" ht="48">
       <c r="B347" s="61">
         <v>24687876</v>
       </c>
@@ -26574,7 +26615,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="348" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="348" spans="1:24" s="144" customFormat="1" ht="36">
       <c r="B348" s="61">
         <v>24687876</v>
       </c>
@@ -26606,7 +26647,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="349" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="349" spans="1:24" s="144" customFormat="1" ht="36">
       <c r="B349" s="61">
         <v>24687876</v>
       </c>
@@ -26702,7 +26743,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="352" spans="1:24" s="144" customFormat="1" ht="24">
+    <row r="352" spans="1:24" s="144" customFormat="1" ht="36">
       <c r="B352" s="61">
         <v>24825607</v>
       </c>
@@ -26741,7 +26782,7 @@
       <c r="C353" s="165" t="s">
         <v>25</v>
       </c>
-      <c r="D353" s="326" t="s">
+      <c r="D353" s="324" t="s">
         <v>1508</v>
       </c>
       <c r="E353" s="61" t="s">
@@ -26773,7 +26814,7 @@
       <c r="C354" s="165" t="s">
         <v>25</v>
       </c>
-      <c r="D354" s="315" t="s">
+      <c r="D354" s="325" t="s">
         <v>1506</v>
       </c>
       <c r="E354" s="61" t="s">
@@ -26805,7 +26846,7 @@
       <c r="C355" s="165" t="s">
         <v>25</v>
       </c>
-      <c r="D355" s="315" t="s">
+      <c r="D355" s="325" t="s">
         <v>1507</v>
       </c>
       <c r="E355" s="61" t="s">
@@ -26830,7 +26871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="356" spans="1:11" s="144" customFormat="1" ht="24">
+    <row r="356" spans="1:11" s="144" customFormat="1" ht="36">
       <c r="B356" s="190">
         <v>24849359</v>
       </c>
@@ -26862,7 +26903,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="357" spans="1:11" s="144" customFormat="1" ht="24">
+    <row r="357" spans="1:11" s="144" customFormat="1" ht="60">
       <c r="B357" s="61">
         <v>24855015</v>
       </c>
@@ -26924,7 +26965,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="359" spans="1:11" s="144" customFormat="1" ht="24">
+    <row r="359" spans="1:11" s="144" customFormat="1" ht="36">
       <c r="B359" s="190">
         <v>24899700</v>
       </c>
@@ -27163,7 +27204,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="366" spans="1:11" s="144" customFormat="1" ht="36">
+    <row r="366" spans="1:11" s="144" customFormat="1" ht="24">
       <c r="A366" s="144" t="s">
         <v>1509</v>
       </c>
@@ -27198,7 +27239,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="367" spans="1:11" s="144" customFormat="1" ht="36">
+    <row r="367" spans="1:11" s="144" customFormat="1" ht="24">
       <c r="A367" s="144" t="s">
         <v>1509</v>
       </c>
@@ -27268,7 +27309,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="369" spans="1:11" s="144" customFormat="1" ht="36">
+    <row r="369" spans="1:11" s="144" customFormat="1" ht="24">
       <c r="A369" s="144" t="s">
         <v>1541</v>
       </c>
@@ -27303,7 +27344,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="370" spans="1:11" s="144" customFormat="1" ht="36">
+    <row r="370" spans="1:11" s="144" customFormat="1" ht="24">
       <c r="A370" s="144" t="s">
         <v>1541</v>
       </c>
@@ -27408,7 +27449,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="373" spans="1:11" s="144" customFormat="1" ht="36">
+    <row r="373" spans="1:11" s="144" customFormat="1" ht="24">
       <c r="A373" s="144" t="s">
         <v>1541</v>
       </c>
@@ -27513,7 +27554,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="376" spans="1:11" s="144" customFormat="1" ht="36">
+    <row r="376" spans="1:11" s="144" customFormat="1" ht="24">
       <c r="A376" s="144" t="s">
         <v>1541</v>
       </c>
@@ -27653,7 +27694,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="380" spans="1:11" s="144" customFormat="1" ht="26">
+    <row r="380" spans="1:11" s="144" customFormat="1" ht="24">
       <c r="A380" s="144" t="s">
         <v>1541</v>
       </c>
@@ -27688,7 +27729,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="381" spans="1:11" s="144" customFormat="1" ht="26">
+    <row r="381" spans="1:11" s="144" customFormat="1" ht="24">
       <c r="A381" s="144" t="s">
         <v>1541</v>
       </c>
@@ -27723,7 +27764,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="382" spans="1:11" s="144" customFormat="1" ht="26">
+    <row r="382" spans="1:11" s="144" customFormat="1" ht="24">
       <c r="A382" s="144" t="s">
         <v>1541</v>
       </c>
@@ -27758,7 +27799,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="383" spans="1:11" s="144" customFormat="1" ht="26">
+    <row r="383" spans="1:11" s="144" customFormat="1" ht="24">
       <c r="A383" s="144" t="s">
         <v>1541</v>
       </c>
@@ -27793,7 +27834,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="384" spans="1:11" s="144" customFormat="1" ht="39">
+    <row r="384" spans="1:11" s="144" customFormat="1" ht="60">
       <c r="B384" s="61">
         <v>24899721</v>
       </c>
@@ -27825,7 +27866,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="385" spans="1:24" s="144" customFormat="1" ht="26">
+    <row r="385" spans="1:24" s="144" customFormat="1" ht="36">
       <c r="B385" s="61">
         <v>24899721</v>
       </c>
@@ -27857,7 +27898,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="386" spans="1:24" s="144" customFormat="1" ht="26">
+    <row r="386" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B386" s="61">
         <v>24899721</v>
       </c>
@@ -27889,7 +27930,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="387" spans="1:24" s="144" customFormat="1" ht="26">
+    <row r="387" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B387" s="61">
         <v>24899721</v>
       </c>
@@ -27921,7 +27962,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="388" spans="1:24" s="144" customFormat="1" ht="26">
+    <row r="388" spans="1:24" s="144" customFormat="1" ht="36">
       <c r="A388" s="292" t="s">
         <v>1510</v>
       </c>
@@ -27969,7 +28010,7 @@
       <c r="W388" s="292"/>
       <c r="X388" s="292"/>
     </row>
-    <row r="389" spans="1:24" s="144" customFormat="1" ht="26">
+    <row r="389" spans="1:24" s="144" customFormat="1" ht="36">
       <c r="B389" s="61">
         <v>24899721</v>
       </c>
@@ -28001,7 +28042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="390" spans="1:24" s="144" customFormat="1" ht="26">
+    <row r="390" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B390" s="61">
         <v>24906209</v>
       </c>
@@ -28033,7 +28074,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="391" spans="1:24" s="144" customFormat="1" ht="48">
+    <row r="391" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B391" s="61">
         <v>24906209</v>
       </c>
@@ -28065,7 +28106,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="392" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="392" spans="1:24" s="144" customFormat="1" ht="13">
       <c r="B392" s="61">
         <v>24906209</v>
       </c>
@@ -28097,7 +28138,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="393" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="393" spans="1:24" s="144" customFormat="1" ht="13">
       <c r="A393" s="292" t="s">
         <v>1505</v>
       </c>
@@ -28145,7 +28186,7 @@
       <c r="W393" s="292"/>
       <c r="X393" s="292"/>
     </row>
-    <row r="394" spans="1:24" s="144" customFormat="1" ht="48">
+    <row r="394" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B394" s="61">
         <v>24920616</v>
       </c>
@@ -28177,7 +28218,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="395" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="395" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B395" s="61">
         <v>24920616</v>
       </c>
@@ -28209,7 +28250,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="396" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="396" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B396" s="61">
         <v>24920616</v>
       </c>
@@ -28241,7 +28282,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="397" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="397" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B397" s="61">
         <v>24920616</v>
       </c>
@@ -28273,7 +28314,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="398" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="398" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B398" s="61">
         <v>24920616</v>
       </c>
@@ -28305,7 +28346,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="399" spans="1:24" s="144" customFormat="1" ht="36">
+    <row r="399" spans="1:24" s="144" customFormat="1" ht="24">
       <c r="B399" s="61">
         <v>24920616</v>
       </c>
@@ -28369,7 +28410,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="401" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="401" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B401" s="61">
         <v>24920619</v>
       </c>
@@ -28401,7 +28442,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="402" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="402" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B402" s="61">
         <v>24920619</v>
       </c>
@@ -28497,7 +28538,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="405" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="405" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B405" s="61">
         <v>24920621</v>
       </c>
@@ -28568,7 +28609,7 @@
       <c r="C407" s="165" t="s">
         <v>25</v>
       </c>
-      <c r="D407" s="319" t="s">
+      <c r="D407" s="312" t="s">
         <v>722</v>
       </c>
       <c r="E407" s="61" t="s">
@@ -28593,14 +28634,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="408" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="408" spans="2:11" s="144" customFormat="1">
       <c r="B408" s="61">
         <v>24954002</v>
       </c>
       <c r="C408" s="165" t="s">
         <v>25</v>
       </c>
-      <c r="D408" s="313" t="s">
+      <c r="D408" s="308" t="s">
         <v>1513</v>
       </c>
       <c r="E408" s="61" t="s">
@@ -28625,7 +28666,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="409" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="409" spans="2:11" s="144" customFormat="1" ht="26">
       <c r="B409" s="61">
         <v>24954002</v>
       </c>
@@ -28657,7 +28698,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="410" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="410" spans="2:11" s="144" customFormat="1" ht="26">
       <c r="B410" s="61">
         <v>24954002</v>
       </c>
@@ -28689,7 +28730,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="411" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="411" spans="2:11" s="144" customFormat="1" ht="26">
       <c r="B411" s="61">
         <v>24954002</v>
       </c>
@@ -28721,7 +28762,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="412" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="412" spans="2:11" s="144" customFormat="1" ht="39">
       <c r="B412" s="61">
         <v>24954002</v>
       </c>
@@ -28753,14 +28794,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="413" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="413" spans="2:11" s="144" customFormat="1">
       <c r="B413" s="61">
         <v>24954002</v>
       </c>
       <c r="C413" s="165" t="s">
         <v>25</v>
       </c>
-      <c r="D413" s="313" t="s">
+      <c r="D413" s="308" t="s">
         <v>1514</v>
       </c>
       <c r="E413" s="61" t="s">
@@ -28785,7 +28826,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="414" spans="2:11" s="144" customFormat="1">
+    <row r="414" spans="2:11" s="144" customFormat="1" ht="48">
       <c r="B414" s="61">
         <v>24956542</v>
       </c>
@@ -28817,7 +28858,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="415" spans="2:11" s="144" customFormat="1">
+    <row r="415" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B415" s="61">
         <v>24956542</v>
       </c>
@@ -28849,7 +28890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="416" spans="2:11" s="144" customFormat="1">
+    <row r="416" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B416" s="61">
         <v>24956542</v>
       </c>
@@ -28881,7 +28922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="417" spans="2:11" s="144" customFormat="1" ht="48">
+    <row r="417" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B417" s="61">
         <v>24956542</v>
       </c>
@@ -28913,7 +28954,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="418" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="418" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B418" s="61">
         <v>24956542</v>
       </c>
@@ -29009,7 +29050,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="421" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="421" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B421" s="61">
         <v>24956542</v>
       </c>
@@ -29041,7 +29082,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="422" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="422" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B422" s="61">
         <v>24956542</v>
       </c>
@@ -29073,7 +29114,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="423" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="423" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B423" s="61">
         <v>24956542</v>
       </c>
@@ -29265,7 +29306,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="429" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="429" spans="2:11" s="144" customFormat="1" ht="48">
       <c r="B429" s="61">
         <v>24956542</v>
       </c>
@@ -29329,14 +29370,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="431" spans="2:11" s="144" customFormat="1" ht="24">
-      <c r="B431" s="313">
+    <row r="431" spans="2:11" s="144" customFormat="1" ht="13">
+      <c r="B431" s="308">
         <v>24990918</v>
       </c>
-      <c r="C431" s="313" t="s">
+      <c r="C431" s="308" t="s">
         <v>2</v>
       </c>
-      <c r="D431" s="320" t="s">
+      <c r="D431" s="313" t="s">
         <v>1516</v>
       </c>
       <c r="E431" s="159" t="s">
@@ -29361,14 +29402,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="432" spans="2:11" s="144" customFormat="1" ht="24">
-      <c r="B432" s="313">
+    <row r="432" spans="2:11" s="144" customFormat="1" ht="13">
+      <c r="B432" s="308">
         <v>24990918</v>
       </c>
-      <c r="C432" s="313" t="s">
+      <c r="C432" s="308" t="s">
         <v>2</v>
       </c>
-      <c r="D432" s="320" t="s">
+      <c r="D432" s="313" t="s">
         <v>1517</v>
       </c>
       <c r="E432" s="159" t="s">
@@ -29393,14 +29434,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="433" spans="2:11" s="144" customFormat="1" ht="24">
-      <c r="B433" s="313">
+    <row r="433" spans="2:11" s="144" customFormat="1" ht="13">
+      <c r="B433" s="308">
         <v>24990918</v>
       </c>
-      <c r="C433" s="313" t="s">
+      <c r="C433" s="308" t="s">
         <v>2</v>
       </c>
-      <c r="D433" s="320" t="s">
+      <c r="D433" s="313" t="s">
         <v>1518</v>
       </c>
       <c r="E433" s="159" t="s">
@@ -29425,14 +29466,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="434" spans="2:11" s="144" customFormat="1" ht="36">
-      <c r="B434" s="313">
+    <row r="434" spans="2:11" s="144" customFormat="1" ht="52">
+      <c r="B434" s="308">
         <v>24990918</v>
       </c>
-      <c r="C434" s="313" t="s">
+      <c r="C434" s="308" t="s">
         <v>2</v>
       </c>
-      <c r="D434" s="322" t="s">
+      <c r="D434" s="315" t="s">
         <v>1519</v>
       </c>
       <c r="E434" s="10" t="s">
@@ -29457,11 +29498,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="435" spans="2:11" s="144" customFormat="1" ht="24">
-      <c r="B435" s="313">
+    <row r="435" spans="2:11" s="144" customFormat="1" ht="36">
+      <c r="B435" s="308">
         <v>24990918</v>
       </c>
-      <c r="C435" s="313" t="s">
+      <c r="C435" s="308" t="s">
         <v>2</v>
       </c>
       <c r="D435" s="172" t="s">
@@ -29489,11 +29530,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="436" spans="2:11" s="144" customFormat="1" ht="36">
-      <c r="B436" s="313">
+    <row r="436" spans="2:11" s="144" customFormat="1" ht="24">
+      <c r="B436" s="308">
         <v>24990918</v>
       </c>
-      <c r="C436" s="313" t="s">
+      <c r="C436" s="308" t="s">
         <v>2</v>
       </c>
       <c r="D436" s="172" t="s">
@@ -29521,7 +29562,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="437" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="437" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B437" s="62">
         <v>25009276</v>
       </c>
@@ -29649,7 +29690,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="441" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="441" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B441" s="61">
         <v>25044230</v>
       </c>
@@ -29681,7 +29722,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="442" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="442" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B442" s="61">
         <v>25044230</v>
       </c>
@@ -29713,7 +29754,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="443" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="443" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B443" s="61">
         <v>25044230</v>
       </c>
@@ -29745,7 +29786,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="444" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="444" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B444" s="183">
         <v>25044230</v>
       </c>
@@ -29777,7 +29818,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="445" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="445" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B445" s="183">
         <v>25044230</v>
       </c>
@@ -30065,7 +30106,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="454" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="454" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B454" s="61">
         <v>25044230</v>
       </c>
@@ -30193,7 +30234,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="458" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="458" spans="2:11" s="144" customFormat="1" ht="36">
       <c r="B458" s="61">
         <v>25048219</v>
       </c>
@@ -30255,7 +30296,7 @@
       </c>
       <c r="K459" s="178"/>
     </row>
-    <row r="460" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="460" spans="2:11" s="144" customFormat="1">
       <c r="B460" s="61">
         <v>25048219</v>
       </c>
@@ -30285,7 +30326,7 @@
       </c>
       <c r="K460" s="178"/>
     </row>
-    <row r="461" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="461" spans="2:11" s="144" customFormat="1">
       <c r="B461" s="61">
         <v>25048219</v>
       </c>
@@ -30315,7 +30356,7 @@
       </c>
       <c r="K461" s="178"/>
     </row>
-    <row r="462" spans="2:11" s="144" customFormat="1" ht="24">
+    <row r="462" spans="2:11" s="144" customFormat="1">
       <c r="B462" s="61">
         <v>25048219</v>
       </c>
@@ -30345,7 +30386,7 @@
       </c>
       <c r="K462" s="178"/>
     </row>
-    <row r="463" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="463" spans="2:11" s="144" customFormat="1" ht="48">
       <c r="B463" s="61">
         <v>25048219</v>
       </c>
@@ -30375,7 +30416,7 @@
       </c>
       <c r="K463" s="178"/>
     </row>
-    <row r="464" spans="2:11" s="144" customFormat="1" ht="48">
+    <row r="464" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B464" s="61">
         <v>25091320</v>
       </c>
@@ -30407,7 +30448,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="465" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="465" spans="2:11" s="144" customFormat="1" ht="24">
       <c r="B465" s="61">
         <v>25091320</v>
       </c>
@@ -30535,14 +30576,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="469" spans="2:11" s="144" customFormat="1" ht="36">
+    <row r="469" spans="2:11" s="144" customFormat="1" ht="26">
       <c r="B469" s="61">
         <v>24715528</v>
       </c>
       <c r="C469" s="165" t="s">
         <v>25</v>
       </c>
-      <c r="D469" s="324" t="s">
+      <c r="D469" s="326" t="s">
         <v>1531</v>
       </c>
       <c r="E469" s="61"/>
@@ -38895,9 +38936,9 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:W930"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G112" sqref="G112"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E110" sqref="E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -45589,16 +45630,16 @@
     </row>
     <row r="26" spans="1:6" s="9" customFormat="1"/>
     <row r="27" spans="1:6">
-      <c r="A27" s="308" t="s">
+      <c r="A27" s="319" t="s">
         <v>961</v>
       </c>
-      <c r="B27" s="308"/>
-      <c r="C27" s="308"/>
-      <c r="D27" s="309" t="s">
+      <c r="B27" s="319"/>
+      <c r="C27" s="319"/>
+      <c r="D27" s="320" t="s">
         <v>962</v>
       </c>
-      <c r="E27" s="310"/>
-      <c r="F27" s="310"/>
+      <c r="E27" s="321"/>
+      <c r="F27" s="321"/>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="18" t="s">
@@ -45799,23 +45840,23 @@
     </row>
     <row r="4" spans="2:13" ht="15">
       <c r="B4" s="44"/>
-      <c r="C4" s="311" t="s">
+      <c r="C4" s="322" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="311"/>
-      <c r="E4" s="311"/>
-      <c r="F4" s="311" t="s">
+      <c r="D4" s="322"/>
+      <c r="E4" s="322"/>
+      <c r="F4" s="322" t="s">
         <v>1350</v>
       </c>
-      <c r="G4" s="311"/>
-      <c r="H4" s="311"/>
-      <c r="I4" s="311"/>
-      <c r="J4" s="311" t="s">
+      <c r="G4" s="322"/>
+      <c r="H4" s="322"/>
+      <c r="I4" s="322"/>
+      <c r="J4" s="322" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="311"/>
-      <c r="L4" s="311"/>
-      <c r="M4" s="311"/>
+      <c r="K4" s="322"/>
+      <c r="L4" s="322"/>
+      <c r="M4" s="322"/>
     </row>
     <row r="5" spans="2:13" ht="16">
       <c r="C5" s="42" t="s">
@@ -46014,41 +46055,41 @@
       </c>
     </row>
     <row r="14" spans="2:13">
-      <c r="C14" s="312" t="s">
+      <c r="C14" s="323" t="s">
         <v>1345</v>
       </c>
-      <c r="D14" s="312"/>
-      <c r="E14" s="312"/>
-      <c r="F14" s="312"/>
-      <c r="G14" s="312"/>
+      <c r="D14" s="323"/>
+      <c r="E14" s="323"/>
+      <c r="F14" s="323"/>
+      <c r="G14" s="323"/>
     </row>
     <row r="15" spans="2:13">
-      <c r="C15" s="312"/>
-      <c r="D15" s="312"/>
-      <c r="E15" s="312"/>
-      <c r="F15" s="312"/>
-      <c r="G15" s="312"/>
+      <c r="C15" s="323"/>
+      <c r="D15" s="323"/>
+      <c r="E15" s="323"/>
+      <c r="F15" s="323"/>
+      <c r="G15" s="323"/>
     </row>
     <row r="16" spans="2:13">
-      <c r="C16" s="312"/>
-      <c r="D16" s="312"/>
-      <c r="E16" s="312"/>
-      <c r="F16" s="312"/>
-      <c r="G16" s="312"/>
+      <c r="C16" s="323"/>
+      <c r="D16" s="323"/>
+      <c r="E16" s="323"/>
+      <c r="F16" s="323"/>
+      <c r="G16" s="323"/>
     </row>
     <row r="17" spans="3:7">
-      <c r="C17" s="312"/>
-      <c r="D17" s="312"/>
-      <c r="E17" s="312"/>
-      <c r="F17" s="312"/>
-      <c r="G17" s="312"/>
+      <c r="C17" s="323"/>
+      <c r="D17" s="323"/>
+      <c r="E17" s="323"/>
+      <c r="F17" s="323"/>
+      <c r="G17" s="323"/>
     </row>
     <row r="18" spans="3:7">
-      <c r="C18" s="312"/>
-      <c r="D18" s="312"/>
-      <c r="E18" s="312"/>
-      <c r="F18" s="312"/>
-      <c r="G18" s="312"/>
+      <c r="C18" s="323"/>
+      <c r="D18" s="323"/>
+      <c r="E18" s="323"/>
+      <c r="F18" s="323"/>
+      <c r="G18" s="323"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>